<commit_message>
Updated README, added requirements.txt for installing dependencies, fixed spreadsheet template, changed request header
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnsonwong/Documents/Projects/Streetwear Sales Tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B985F2-85A8-8E4F-AF88-E2E7D5FF8D3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FFC2DF-BE2F-F245-8603-D449407B9395}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
     <t>Supreme Shoulder Bag (Black) SS18</t>
   </si>
   <si>
-    <t>asd</t>
+    <t>StockX Price</t>
   </si>
 </sst>
 </file>
@@ -319,7 +319,8 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -327,7 +328,7 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thick">
+        <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
@@ -354,6 +355,24 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -362,6 +381,59 @@
           <color indexed="64"/>
         </right>
         <top style="thick">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thick">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
@@ -380,6 +452,24 @@
           <color indexed="64"/>
         </right>
         <top style="thick">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
@@ -407,6 +497,24 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -415,6 +523,24 @@
           <color indexed="64"/>
         </right>
         <top style="thick">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
@@ -440,6 +566,24 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -449,6 +593,23 @@
           <color indexed="64"/>
         </right>
         <top style="thick">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
@@ -481,167 +642,6 @@
           <color indexed="64"/>
         </right>
         <top style="thick">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
@@ -783,26 +783,26 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="template" displayName="template" ref="A1:J5" totalsRowCount="1" headerRowDxfId="25" dataDxfId="23" totalsRowDxfId="21" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="20">
   <autoFilter ref="A1:J4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
       <totalsRowFormula>"Total Items: " &amp; SUBTOTAL(103,template[Item])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Size" dataDxfId="18" totalsRowDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="StockX Ticker Symbol" dataDxfId="17" totalsRowDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Price Paid" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Profit" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="5">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Size" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="StockX Ticker Symbol" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Price Paid" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Profit" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>G2-D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Profit %" totalsRowFunction="average" dataDxfId="14" totalsRowDxfId="4">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Profit %" totalsRowFunction="average" dataDxfId="9" totalsRowDxfId="8">
       <calculatedColumnFormula>(E2/D2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="asd" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="StockX Payout" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="2">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="StockX Price" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="StockX Payout" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4">
       <calculatedColumnFormula>G2*0.89</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="StockX Profit" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="1">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="StockX Profit" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2">
       <calculatedColumnFormula>H2-D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="StockX Profit %" totalsRowFunction="average" dataDxfId="10" totalsRowDxfId="0">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="StockX Profit %" totalsRowFunction="average" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>I2/D2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1115,7 +1115,7 @@
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A28" sqref="A28:XFD28"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1342,7 +1342,7 @@
         <v>-1</v>
       </c>
       <c r="G5" s="7">
-        <f>SUBTOTAL(109,template[asd])</f>
+        <f>SUBTOTAL(109,template[StockX Price])</f>
         <v>0</v>
       </c>
       <c r="H5" s="7">

</xml_diff>

<commit_message>
changed request header and update price logic
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnsonwong/Documents/Projects/Streetwear Sales Tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FFC2DF-BE2F-F245-8603-D449407B9395}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35545CA9-A7D2-BA45-8A7D-B56503770275}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1115,7 +1115,7 @@
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A28" sqref="A28:XFD28"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>